<commit_message>
Suites module xpath changes
</commit_message>
<xml_diff>
--- a/src/test/resources/Excel/TestDatas.xlsx
+++ b/src/test/resources/Excel/TestDatas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6910" activeTab="2"/>
+    <workbookView windowWidth="19200" windowHeight="6950"/>
   </bookViews>
   <sheets>
     <sheet name="Environments" sheetId="1" r:id="rId1"/>
@@ -17,32 +17,90 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
   <si>
     <t>Environments</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>https://qa.xealei.com/</t>
+  </si>
+  <si>
+    <t>PRE-POD</t>
+  </si>
+  <si>
+    <t>https://preprod.xealei.com/login</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>fa@xealei.com</t>
+  </si>
+  <si>
+    <t>xealei@23</t>
   </si>
   <si>
     <r>
       <rPr>
-        <sz val="12"/>
-        <color rgb="FF2A00FF"/>
-        <rFont val="Consolas"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
         <charset val="134"/>
+        <scheme val="minor"/>
       </rPr>
-      <t>https://qa.xealei.com/</t>
+      <t>alphindadmin@xealei.com</t>
     </r>
   </si>
   <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>fa@xealei.com</t>
-  </si>
-  <si>
-    <t>xealei@23</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>A!ph!nd@dm!n</t>
+    </r>
+  </si>
+  <si>
+    <t>ALPHIND</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ghaadmin@xealei.com</t>
+    </r>
+  </si>
+  <si>
+    <t>GHA</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>xliadmin@xealei.com</t>
+    </r>
+  </si>
+  <si>
+    <t>XEALEI</t>
   </si>
   <si>
     <t>SuiteName</t>
@@ -81,7 +139,7 @@
     <t>12</t>
   </si>
   <si>
-    <t>Suite-16:43:30</t>
+    <t>Suite-12:10:37</t>
   </si>
   <si>
     <t>Available</t>
@@ -108,7 +166,7 @@
     <t>10</t>
   </si>
   <si>
-    <t>Royal-16:40:40</t>
+    <t>Royal-12:10:54</t>
   </si>
   <si>
     <t>Active</t>
@@ -117,46 +175,19 @@
     <t>In-Active</t>
   </si>
   <si>
-    <t>Suite-16:45:07</t>
-  </si>
-  <si>
-    <t>Royal-16:45:33</t>
-  </si>
-  <si>
-    <t>Suite-16:47:38</t>
-  </si>
-  <si>
-    <t>Royal-16:47:55</t>
-  </si>
-  <si>
-    <t>Suite-17:03:29</t>
-  </si>
-  <si>
-    <t>Royal-17:03:45</t>
-  </si>
-  <si>
-    <t>Suite-19:19:19</t>
-  </si>
-  <si>
-    <t>Royal-19:19:49</t>
-  </si>
-  <si>
-    <t>Suite-19:21:19</t>
-  </si>
-  <si>
-    <t>Royal-19:21:38</t>
-  </si>
-  <si>
-    <t>Suite-19:23:27</t>
-  </si>
-  <si>
-    <t>Royal-19:23:46</t>
+    <t>Suite-13:20:05</t>
+  </si>
+  <si>
+    <t>Suite-14:37:33</t>
+  </si>
+  <si>
+    <t>Royal-14:37:51</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -213,24 +244,24 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF2A00FF"/>
-      <name val="Consolas"/>
-      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -569,7 +600,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -603,6 +634,19 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -721,13 +765,13 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -739,34 +783,34 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -851,7 +895,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -876,9 +920,15 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="6" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" quotePrefix="1"/>
   </cellXfs>
@@ -1200,28 +1250,55 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="5" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="28.5454545454545"/>
+    <col min="1" max="1" customWidth="true" width="17.3636363636364"/>
+    <col min="2" max="2" customWidth="true" width="29.0909090909091"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" ht="15.5" spans="1:1">
-      <c r="A2" s="16" t="s">
+    <row r="2" ht="15.5" spans="1:2">
+      <c r="A2" s="18" t="s">
         <v>1</v>
       </c>
+      <c r="B2" s="8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="16"/>
+      <c r="B4" s="16"/>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="16"/>
+      <c r="B6" s="16"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" display="https://preprod.xealei.com/login" tooltip="https://preprod.xealei.com/login"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
@@ -1230,32 +1307,66 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5" outlineLevelRow="4" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.0"/>
-    <col min="2" max="2" customWidth="true" width="11.4545454545455"/>
+    <col min="1" max="1" customWidth="true" width="23.7272727272727"/>
+    <col min="2" max="2" customWidth="true" width="15.2727272727273"/>
+    <col min="3" max="3" customWidth="true" width="9.18181818181818"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="13" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="14" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>5</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -1273,7 +1384,7 @@
   <sheetPr/>
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -1289,48 +1400,48 @@
   <sheetData>
     <row r="1" s="11" customFormat="1" ht="18" spans="1:7">
       <c r="A1" s="4" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" ht="15.5" spans="1:7">
       <c r="A2" s="9" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>17</v>
+        <v>24</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1358,53 +1469,53 @@
   <sheetData>
     <row r="1" ht="15" spans="1:7">
       <c r="A1" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" ht="15.5" spans="1:7">
       <c r="A2" s="7" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>26</v>
+        <v>33</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>36</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="7:7">
       <c r="G3" s="7" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>